<commit_message>
add results and new trained models, add result graphs
</commit_message>
<xml_diff>
--- a/docs/selected_features2.xlsx
+++ b/docs/selected_features2.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raidel\Documents\School\FSU\Grad\Graduation_Project\AlzheTect\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{416B7BB1-6223-4003-8BBD-8BC6001B9F14}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A61A1F-2228-4723-A787-61B10B7C729C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15450" windowHeight="7140" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15450" windowHeight="7140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="selected_features" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
   <si>
     <t>Field_Name</t>
   </si>
@@ -159,13 +159,16 @@
   </si>
   <si>
     <t>Total Fields: 20</t>
+  </si>
+  <si>
+    <t>Table 3: Selected Features using the random forest classifier, along with the keys for the featuresi n the dataset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,6 +299,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -734,7 +744,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -748,10 +758,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -834,13 +847,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="double">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -851,6 +857,13 @@
           <color indexed="64"/>
         </top>
         <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
           <color indexed="64"/>
         </bottom>
       </border>
@@ -898,11 +911,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:B21" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="2" tableBorderDxfId="3">
-  <autoFilter ref="A1:B21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="A1:B21" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
+  <autoFilter ref="A1:B21" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Measurement_Type" dataDxfId="1"/>
-    <tableColumn id="2" name="Field_Name" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Measurement_Type" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Field_Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1204,7 +1217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1416,14 +1429,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1602,17 +1615,24 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="9"/>
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="95" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="93" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>